<commit_message>
Subindo ajustes de mer e remapeamento de db
</commit_message>
<xml_diff>
--- a/analise/Gerenciamento.xlsx
+++ b/analise/Gerenciamento.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\Desktop\TCC\analise\casos de uso\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\Desktop\TCC\analise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5914D6B6-9F43-4155-972B-337EC83F4834}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84DF9529-B783-421F-89EB-3723E940A5A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requisitos" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="103">
   <si>
     <t>Modulo</t>
   </si>
@@ -297,6 +297,51 @@
   </si>
   <si>
     <t>Nome Atividade</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>Inserir Anúncio</t>
+  </si>
+  <si>
+    <t>Cadastrar Funcionario</t>
+  </si>
+  <si>
+    <t>Carrinho</t>
+  </si>
+  <si>
+    <t>Finalizar Comprar</t>
+  </si>
+  <si>
+    <t>Cancelar conta</t>
+  </si>
+  <si>
+    <t>Devolução</t>
+  </si>
+  <si>
+    <t>Comfirmar Devolução - Funcionario</t>
+  </si>
+  <si>
+    <t>Esqueci a Senha</t>
+  </si>
+  <si>
+    <t>Minhas Comprar</t>
+  </si>
+  <si>
+    <t>Cancelar Pedido</t>
+  </si>
+  <si>
+    <t>Alterar Dados - Cliente</t>
+  </si>
+  <si>
+    <t>Favoritos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perfil/Endereço </t>
   </si>
 </sst>
 </file>
@@ -654,7 +699,7 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -740,82 +785,79 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="9" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="10" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="9" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="10" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="10" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="14" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2152,7 +2194,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18:A20"/>
     </sheetView>
   </sheetViews>
@@ -2191,7 +2233,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="47" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -2212,7 +2254,7 @@
       <c r="G2" s="12"/>
     </row>
     <row r="3" spans="1:7" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="37"/>
+      <c r="A3" s="47"/>
       <c r="B3" s="7" t="s">
         <v>9</v>
       </c>
@@ -2231,7 +2273,7 @@
       <c r="G3" s="12"/>
     </row>
     <row r="4" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="37"/>
+      <c r="A4" s="47"/>
       <c r="B4" s="14" t="s">
         <v>26</v>
       </c>
@@ -2250,7 +2292,7 @@
       <c r="G4" s="12"/>
     </row>
     <row r="5" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="37"/>
+      <c r="A5" s="47"/>
       <c r="B5" s="18" t="s">
         <v>21</v>
       </c>
@@ -2269,7 +2311,7 @@
       <c r="G5" s="12"/>
     </row>
     <row r="6" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="37"/>
+      <c r="A6" s="47"/>
       <c r="B6" s="18" t="s">
         <v>23</v>
       </c>
@@ -2288,7 +2330,7 @@
       <c r="G6" s="12"/>
     </row>
     <row r="7" spans="1:7" ht="95.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="47" t="s">
         <v>27</v>
       </c>
       <c r="B7" s="7" t="s">
@@ -2309,7 +2351,7 @@
       <c r="G7" s="12"/>
     </row>
     <row r="8" spans="1:7" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="37"/>
+      <c r="A8" s="47"/>
       <c r="B8" s="7" t="s">
         <v>30</v>
       </c>
@@ -2328,7 +2370,7 @@
       <c r="G8" s="12"/>
     </row>
     <row r="9" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="37"/>
+      <c r="A9" s="47"/>
       <c r="B9" s="14" t="s">
         <v>32</v>
       </c>
@@ -2347,7 +2389,7 @@
       <c r="G9" s="12"/>
     </row>
     <row r="10" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="37"/>
+      <c r="A10" s="47"/>
       <c r="B10" s="18" t="s">
         <v>34</v>
       </c>
@@ -2366,7 +2408,7 @@
       <c r="G10" s="12"/>
     </row>
     <row r="11" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="37"/>
+      <c r="A11" s="47"/>
       <c r="B11" s="18" t="s">
         <v>36</v>
       </c>
@@ -2385,7 +2427,7 @@
       <c r="G11" s="12"/>
     </row>
     <row r="12" spans="1:7" ht="95.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="47" t="s">
         <v>38</v>
       </c>
       <c r="B12" s="7" t="s">
@@ -2406,7 +2448,7 @@
       <c r="G12" s="12"/>
     </row>
     <row r="13" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="37"/>
+      <c r="A13" s="47"/>
       <c r="B13" s="14" t="s">
         <v>40</v>
       </c>
@@ -2425,7 +2467,7 @@
       <c r="G13" s="12"/>
     </row>
     <row r="14" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="37"/>
+      <c r="A14" s="47"/>
       <c r="B14" s="18" t="s">
         <v>41</v>
       </c>
@@ -2444,7 +2486,7 @@
       <c r="G14" s="12"/>
     </row>
     <row r="15" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="37"/>
+      <c r="A15" s="47"/>
       <c r="B15" s="18" t="s">
         <v>42</v>
       </c>
@@ -2463,7 +2505,7 @@
       <c r="G15" s="12"/>
     </row>
     <row r="16" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="37"/>
+      <c r="A16" s="47"/>
       <c r="B16" s="18" t="s">
         <v>43</v>
       </c>
@@ -2482,7 +2524,7 @@
       <c r="G16" s="12"/>
     </row>
     <row r="17" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="37"/>
+      <c r="A17" s="47"/>
       <c r="B17" s="14" t="s">
         <v>44</v>
       </c>
@@ -2501,7 +2543,7 @@
       <c r="G17" s="12"/>
     </row>
     <row r="18" spans="1:7" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="37" t="s">
+      <c r="A18" s="47" t="s">
         <v>53</v>
       </c>
       <c r="B18" s="7" t="s">
@@ -2522,7 +2564,7 @@
       <c r="G18" s="12"/>
     </row>
     <row r="19" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="37"/>
+      <c r="A19" s="47"/>
       <c r="B19" s="14" t="s">
         <v>55</v>
       </c>
@@ -2541,7 +2583,7 @@
       <c r="G19" s="12"/>
     </row>
     <row r="20" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="37"/>
+      <c r="A20" s="47"/>
       <c r="B20" s="14" t="s">
         <v>56</v>
       </c>
@@ -2560,10 +2602,10 @@
       <c r="G20" s="12"/>
     </row>
     <row r="21" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="40" t="s">
+      <c r="A21" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="41"/>
+      <c r="B21" s="51"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="22"/>
@@ -2587,10 +2629,10 @@
       <c r="A25" s="26"/>
     </row>
     <row r="26" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A26" s="38" t="s">
+      <c r="A26" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="39"/>
+      <c r="B26" s="49"/>
     </row>
     <row r="27" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A27" s="27">
@@ -2686,31 +2728,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E3E3989-44EE-421D-BBD1-34EC265F0F69}">
-  <dimension ref="A1:F339"/>
+  <dimension ref="A1:F340"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" thickBottom="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.85546875" style="36" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" style="36" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" style="36" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="48.42578125" style="36" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" style="48" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" style="38" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.85546875" style="36" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="56" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
     </row>
     <row r="2" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="35" t="s">
@@ -2725,7 +2767,7 @@
       <c r="D2" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="E2" s="59" t="s">
+      <c r="E2" s="43" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="35" t="s">
@@ -2733,187 +2775,187 @@
       </c>
     </row>
     <row r="3" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="49">
+      <c r="A3" s="57">
         <v>1</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="52">
+        <v>44121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="54"/>
+      <c r="B4" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="53"/>
+    </row>
+    <row r="5" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="57">
+        <v>2</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" s="52">
+        <v>44123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="54"/>
+      <c r="B6" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" s="54"/>
+    </row>
+    <row r="7" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="55"/>
+      <c r="B7" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" s="55"/>
+    </row>
+    <row r="8" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="57">
+        <v>3</v>
+      </c>
+      <c r="B8" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" s="52">
+        <v>44125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="54"/>
+      <c r="B9" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="D9" s="54"/>
+    </row>
+    <row r="10" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="55"/>
+      <c r="B10" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="D10" s="55"/>
+    </row>
+    <row r="11" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="57">
+        <v>4</v>
+      </c>
+      <c r="B11" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="D11" s="52">
+        <v>44127</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="54"/>
+      <c r="B12" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="D3" s="53">
-        <v>44121</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="51"/>
-      <c r="B4" s="52" t="s">
+      <c r="D12" s="54"/>
+    </row>
+    <row r="13" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="55"/>
+      <c r="B13" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13" s="55"/>
+    </row>
+    <row r="14" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="57">
+        <v>5</v>
+      </c>
+      <c r="B14" s="39" t="s">
+        <v>102</v>
+      </c>
+      <c r="D14" s="52">
+        <v>44129</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="54"/>
+      <c r="B15" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="D4" s="54"/>
-    </row>
-    <row r="5" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="50"/>
-      <c r="B5" s="52" t="s">
+      <c r="D15" s="54"/>
+    </row>
+    <row r="16" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="55"/>
+      <c r="B16" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="D5" s="55"/>
-    </row>
-    <row r="6" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="49">
-        <v>2</v>
-      </c>
-      <c r="B6" s="52" t="s">
-        <v>87</v>
-      </c>
-      <c r="D6" s="53">
-        <v>44123</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="51"/>
-      <c r="B7" s="52" t="s">
-        <v>87</v>
-      </c>
-      <c r="D7" s="51"/>
-    </row>
-    <row r="8" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="50"/>
-      <c r="B8" s="52" t="s">
-        <v>87</v>
-      </c>
-      <c r="D8" s="50"/>
-    </row>
-    <row r="9" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="49">
-        <v>3</v>
-      </c>
-      <c r="B9" s="52" t="s">
-        <v>87</v>
-      </c>
-      <c r="D9" s="53">
-        <v>44125</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="51"/>
-      <c r="B10" s="52" t="s">
-        <v>87</v>
-      </c>
-      <c r="D10" s="51"/>
-    </row>
-    <row r="11" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="50"/>
-      <c r="B11" s="52" t="s">
-        <v>87</v>
-      </c>
-      <c r="D11" s="50"/>
-    </row>
-    <row r="12" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="49">
-        <v>4</v>
-      </c>
-      <c r="B12" s="52" t="s">
-        <v>87</v>
-      </c>
-      <c r="D12" s="53">
-        <v>44127</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="51"/>
-      <c r="B13" s="52" t="s">
-        <v>87</v>
-      </c>
-      <c r="D13" s="51"/>
-    </row>
-    <row r="14" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="50"/>
-      <c r="B14" s="52" t="s">
-        <v>87</v>
-      </c>
-      <c r="D14" s="50"/>
-    </row>
-    <row r="15" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="49">
-        <v>5</v>
-      </c>
-      <c r="B15" s="52" t="s">
-        <v>87</v>
-      </c>
-      <c r="D15" s="53">
-        <v>44129</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="51"/>
-      <c r="B16" s="52" t="s">
-        <v>87</v>
-      </c>
-      <c r="D16" s="51"/>
+      <c r="D16" s="55"/>
     </row>
     <row r="17" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="50"/>
-      <c r="B17" s="52" t="s">
-        <v>87</v>
-      </c>
-      <c r="D17" s="50"/>
+      <c r="A17" s="57">
+        <v>6</v>
+      </c>
+      <c r="B17" s="39" t="s">
+        <v>101</v>
+      </c>
+      <c r="D17" s="52">
+        <v>44131</v>
+      </c>
     </row>
     <row r="18" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="49">
-        <v>6</v>
-      </c>
-      <c r="B18" s="52" t="s">
-        <v>87</v>
-      </c>
-      <c r="D18" s="53">
-        <v>44131</v>
-      </c>
+      <c r="A18" s="54"/>
+      <c r="B18" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="D18" s="54"/>
     </row>
     <row r="19" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="51"/>
-      <c r="B19" s="52" t="s">
-        <v>87</v>
-      </c>
-      <c r="D19" s="51"/>
+      <c r="A19" s="55"/>
+      <c r="B19" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19" s="55"/>
     </row>
     <row r="20" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="50"/>
-      <c r="B20" s="52" t="s">
-        <v>87</v>
-      </c>
-      <c r="D20" s="50"/>
+      <c r="A20" s="57">
+        <v>7</v>
+      </c>
+      <c r="B20" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="D20" s="52">
+        <v>44133</v>
+      </c>
     </row>
     <row r="21" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="49">
-        <v>7</v>
-      </c>
-      <c r="B21" s="52" t="s">
-        <v>87</v>
-      </c>
-      <c r="D21" s="53">
-        <v>44133</v>
-      </c>
+      <c r="A21" s="54"/>
+      <c r="B21" s="39" t="s">
+        <v>95</v>
+      </c>
+      <c r="D21" s="53"/>
     </row>
     <row r="22" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="50"/>
-      <c r="B22" s="52" t="s">
-        <v>87</v>
-      </c>
-      <c r="D22" s="50"/>
+      <c r="A22" s="55"/>
+      <c r="B22" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="D22" s="55"/>
     </row>
     <row r="23" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="57">
+      <c r="A23" s="41">
         <v>8</v>
       </c>
-      <c r="B23" s="52" t="s">
+      <c r="B23" s="39" t="s">
         <v>81</v>
       </c>
       <c r="C23" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="D23" s="58">
+      <c r="D23" s="42">
         <v>44135</v>
       </c>
-      <c r="E23" s="48" t="s">
+      <c r="E23" s="38" t="s">
         <v>83</v>
       </c>
       <c r="F23" s="36" t="s">
@@ -2921,964 +2963,965 @@
       </c>
     </row>
     <row r="24" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D24" s="56"/>
+      <c r="D24" s="40"/>
     </row>
     <row r="25" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D25" s="56"/>
+      <c r="D25" s="40"/>
     </row>
     <row r="26" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D26" s="56"/>
+      <c r="D26" s="40"/>
     </row>
     <row r="27" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D27" s="56"/>
+      <c r="D27" s="40"/>
     </row>
     <row r="28" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D28" s="56"/>
+      <c r="D28" s="40"/>
     </row>
     <row r="29" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D29" s="56"/>
+      <c r="D29" s="40"/>
     </row>
     <row r="30" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D30" s="56"/>
+      <c r="D30" s="40"/>
     </row>
     <row r="31" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D31" s="56"/>
+      <c r="D31" s="40"/>
     </row>
     <row r="32" spans="1:6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="56"/>
+      <c r="D32" s="40"/>
     </row>
     <row r="33" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D33" s="56"/>
+      <c r="D33" s="40"/>
     </row>
     <row r="34" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D34" s="56"/>
+      <c r="D34" s="40"/>
     </row>
     <row r="35" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D35" s="56"/>
+      <c r="D35" s="40"/>
     </row>
     <row r="36" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D36" s="56"/>
+      <c r="D36" s="40"/>
     </row>
     <row r="37" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D37" s="56"/>
+      <c r="D37" s="40"/>
     </row>
     <row r="38" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D38" s="56"/>
+      <c r="D38" s="40"/>
     </row>
     <row r="39" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D39" s="56"/>
+      <c r="D39" s="40"/>
     </row>
     <row r="40" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D40" s="56"/>
+      <c r="D40" s="40"/>
     </row>
     <row r="41" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D41" s="56"/>
+      <c r="D41" s="40"/>
     </row>
     <row r="42" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D42" s="56"/>
+      <c r="D42" s="40"/>
     </row>
     <row r="43" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D43" s="56"/>
+      <c r="D43" s="40"/>
     </row>
     <row r="44" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D44" s="56"/>
+      <c r="D44" s="40"/>
     </row>
     <row r="45" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D45" s="56"/>
+      <c r="D45" s="40"/>
     </row>
     <row r="46" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D46" s="56"/>
+      <c r="D46" s="40"/>
     </row>
     <row r="47" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D47" s="56"/>
+      <c r="D47" s="40"/>
     </row>
     <row r="48" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D48" s="56"/>
+      <c r="D48" s="40"/>
     </row>
     <row r="49" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D49" s="56"/>
+      <c r="D49" s="40"/>
     </row>
     <row r="50" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D50" s="56"/>
+      <c r="D50" s="40"/>
     </row>
     <row r="51" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D51" s="56"/>
+      <c r="D51" s="40"/>
     </row>
     <row r="52" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D52" s="56"/>
+      <c r="D52" s="40"/>
     </row>
     <row r="53" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D53" s="56"/>
+      <c r="D53" s="40"/>
     </row>
     <row r="54" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D54" s="56"/>
+      <c r="D54" s="40"/>
     </row>
     <row r="55" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D55" s="56"/>
+      <c r="D55" s="40"/>
     </row>
     <row r="56" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D56" s="56"/>
+      <c r="D56" s="40"/>
     </row>
     <row r="57" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D57" s="56"/>
+      <c r="D57" s="40"/>
     </row>
     <row r="58" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D58" s="56"/>
+      <c r="D58" s="40"/>
     </row>
     <row r="59" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D59" s="56"/>
+      <c r="D59" s="40"/>
     </row>
     <row r="60" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D60" s="56"/>
+      <c r="D60" s="40"/>
     </row>
     <row r="61" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D61" s="56"/>
+      <c r="D61" s="40"/>
     </row>
     <row r="62" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D62" s="56"/>
+      <c r="D62" s="40"/>
     </row>
     <row r="63" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D63" s="56"/>
+      <c r="D63" s="40"/>
     </row>
     <row r="64" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D64" s="56"/>
+      <c r="D64" s="40"/>
     </row>
     <row r="65" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D65" s="56"/>
+      <c r="D65" s="40"/>
     </row>
     <row r="66" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D66" s="56"/>
+      <c r="D66" s="40"/>
     </row>
     <row r="67" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D67" s="56"/>
+      <c r="D67" s="40"/>
     </row>
     <row r="68" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D68" s="56"/>
+      <c r="D68" s="40"/>
     </row>
     <row r="69" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D69" s="56"/>
+      <c r="D69" s="40"/>
     </row>
     <row r="70" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D70" s="56"/>
+      <c r="D70" s="40"/>
     </row>
     <row r="71" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D71" s="56"/>
+      <c r="D71" s="40"/>
     </row>
     <row r="72" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D72" s="56"/>
+      <c r="D72" s="40"/>
     </row>
     <row r="73" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D73" s="56"/>
+      <c r="D73" s="40"/>
     </row>
     <row r="74" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D74" s="56"/>
+      <c r="D74" s="40"/>
     </row>
     <row r="75" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D75" s="56"/>
+      <c r="D75" s="40"/>
     </row>
     <row r="76" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D76" s="56"/>
+      <c r="D76" s="40"/>
     </row>
     <row r="77" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D77" s="56"/>
+      <c r="D77" s="40"/>
     </row>
     <row r="78" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D78" s="56"/>
+      <c r="D78" s="40"/>
     </row>
     <row r="79" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D79" s="56"/>
+      <c r="D79" s="40"/>
     </row>
     <row r="80" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D80" s="56"/>
+      <c r="D80" s="40"/>
     </row>
     <row r="81" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D81" s="56"/>
+      <c r="D81" s="40"/>
     </row>
     <row r="82" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D82" s="56"/>
+      <c r="D82" s="40"/>
     </row>
     <row r="83" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D83" s="56"/>
+      <c r="D83" s="40"/>
     </row>
     <row r="84" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D84" s="56"/>
+      <c r="D84" s="40"/>
     </row>
     <row r="85" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D85" s="56"/>
+      <c r="D85" s="40"/>
     </row>
     <row r="86" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D86" s="56"/>
+      <c r="D86" s="40"/>
     </row>
     <row r="87" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D87" s="56"/>
+      <c r="D87" s="40"/>
     </row>
     <row r="88" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D88" s="56"/>
+      <c r="D88" s="40"/>
     </row>
     <row r="89" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D89" s="56"/>
+      <c r="D89" s="40"/>
     </row>
     <row r="90" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D90" s="56"/>
+      <c r="D90" s="40"/>
     </row>
     <row r="91" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D91" s="56"/>
+      <c r="D91" s="40"/>
     </row>
     <row r="92" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D92" s="56"/>
+      <c r="D92" s="40"/>
     </row>
     <row r="93" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D93" s="56"/>
+      <c r="D93" s="40"/>
     </row>
     <row r="94" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D94" s="56"/>
+      <c r="D94" s="40"/>
     </row>
     <row r="95" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D95" s="56"/>
+      <c r="D95" s="40"/>
     </row>
     <row r="96" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D96" s="56"/>
+      <c r="D96" s="40"/>
     </row>
     <row r="97" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D97" s="56"/>
+      <c r="D97" s="40"/>
     </row>
     <row r="98" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D98" s="56"/>
+      <c r="D98" s="40"/>
     </row>
     <row r="99" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D99" s="56"/>
+      <c r="D99" s="40"/>
     </row>
     <row r="100" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D100" s="56"/>
+      <c r="D100" s="40"/>
     </row>
     <row r="101" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D101" s="56"/>
+      <c r="D101" s="40"/>
     </row>
     <row r="102" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D102" s="56"/>
+      <c r="D102" s="40"/>
     </row>
     <row r="103" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D103" s="56"/>
+      <c r="D103" s="40"/>
     </row>
     <row r="104" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D104" s="56"/>
+      <c r="D104" s="40"/>
     </row>
     <row r="105" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D105" s="56"/>
+      <c r="D105" s="40"/>
     </row>
     <row r="106" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D106" s="56"/>
+      <c r="D106" s="40"/>
     </row>
     <row r="107" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D107" s="56"/>
+      <c r="D107" s="40"/>
     </row>
     <row r="108" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D108" s="56"/>
+      <c r="D108" s="40"/>
     </row>
     <row r="109" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D109" s="56"/>
+      <c r="D109" s="40"/>
     </row>
     <row r="110" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D110" s="56"/>
+      <c r="D110" s="40"/>
     </row>
     <row r="111" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D111" s="56"/>
+      <c r="D111" s="40"/>
     </row>
     <row r="112" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D112" s="56"/>
+      <c r="D112" s="40"/>
     </row>
     <row r="113" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D113" s="56"/>
+      <c r="D113" s="40"/>
     </row>
     <row r="114" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D114" s="56"/>
+      <c r="D114" s="40"/>
     </row>
     <row r="115" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D115" s="56"/>
+      <c r="D115" s="40"/>
     </row>
     <row r="116" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D116" s="56"/>
+      <c r="D116" s="40"/>
     </row>
     <row r="117" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D117" s="56"/>
+      <c r="D117" s="40"/>
     </row>
     <row r="118" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D118" s="56"/>
+      <c r="D118" s="40"/>
     </row>
     <row r="119" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D119" s="56"/>
+      <c r="D119" s="40"/>
     </row>
     <row r="120" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D120" s="56"/>
+      <c r="D120" s="40"/>
     </row>
     <row r="121" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D121" s="56"/>
+      <c r="D121" s="40"/>
     </row>
     <row r="122" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D122" s="56"/>
+      <c r="D122" s="40"/>
     </row>
     <row r="123" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D123" s="56"/>
+      <c r="D123" s="40"/>
     </row>
     <row r="124" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D124" s="56"/>
+      <c r="D124" s="40"/>
     </row>
     <row r="125" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D125" s="56"/>
+      <c r="D125" s="40"/>
     </row>
     <row r="126" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D126" s="56"/>
+      <c r="D126" s="40"/>
     </row>
     <row r="127" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D127" s="56"/>
+      <c r="D127" s="40"/>
     </row>
     <row r="128" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D128" s="56"/>
+      <c r="D128" s="40"/>
     </row>
     <row r="129" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D129" s="56"/>
+      <c r="D129" s="40"/>
     </row>
     <row r="130" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D130" s="56"/>
+      <c r="D130" s="40"/>
     </row>
     <row r="131" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D131" s="56"/>
+      <c r="D131" s="40"/>
     </row>
     <row r="132" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D132" s="56"/>
+      <c r="D132" s="40"/>
     </row>
     <row r="133" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D133" s="56"/>
+      <c r="D133" s="40"/>
     </row>
     <row r="134" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D134" s="56"/>
+      <c r="D134" s="40"/>
     </row>
     <row r="135" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D135" s="56"/>
+      <c r="D135" s="40"/>
     </row>
     <row r="136" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D136" s="56"/>
+      <c r="D136" s="40"/>
     </row>
     <row r="137" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D137" s="56"/>
+      <c r="D137" s="40"/>
     </row>
     <row r="138" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D138" s="56"/>
+      <c r="D138" s="40"/>
     </row>
     <row r="139" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D139" s="56"/>
+      <c r="D139" s="40"/>
     </row>
     <row r="140" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D140" s="56"/>
+      <c r="D140" s="40"/>
     </row>
     <row r="141" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D141" s="56"/>
+      <c r="D141" s="40"/>
     </row>
     <row r="142" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D142" s="56"/>
+      <c r="D142" s="40"/>
     </row>
     <row r="143" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D143" s="56"/>
+      <c r="D143" s="40"/>
     </row>
     <row r="144" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D144" s="56"/>
+      <c r="D144" s="40"/>
     </row>
     <row r="145" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D145" s="56"/>
+      <c r="D145" s="40"/>
     </row>
     <row r="146" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D146" s="56"/>
+      <c r="D146" s="40"/>
     </row>
     <row r="147" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D147" s="56"/>
+      <c r="D147" s="40"/>
     </row>
     <row r="148" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D148" s="56"/>
+      <c r="D148" s="40"/>
     </row>
     <row r="149" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D149" s="56"/>
+      <c r="D149" s="40"/>
     </row>
     <row r="150" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D150" s="56"/>
+      <c r="D150" s="40"/>
     </row>
     <row r="151" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D151" s="56"/>
+      <c r="D151" s="40"/>
     </row>
     <row r="152" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D152" s="56"/>
+      <c r="D152" s="40"/>
     </row>
     <row r="153" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D153" s="56"/>
+      <c r="D153" s="40"/>
     </row>
     <row r="154" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D154" s="56"/>
+      <c r="D154" s="40"/>
     </row>
     <row r="155" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D155" s="56"/>
+      <c r="D155" s="40"/>
     </row>
     <row r="156" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D156" s="56"/>
+      <c r="D156" s="40"/>
     </row>
     <row r="157" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D157" s="56"/>
+      <c r="D157" s="40"/>
     </row>
     <row r="158" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D158" s="56"/>
+      <c r="D158" s="40"/>
     </row>
     <row r="159" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D159" s="56"/>
+      <c r="D159" s="40"/>
     </row>
     <row r="160" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D160" s="56"/>
+      <c r="D160" s="40"/>
     </row>
     <row r="161" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D161" s="56"/>
+      <c r="D161" s="40"/>
     </row>
     <row r="162" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D162" s="56"/>
+      <c r="D162" s="40"/>
     </row>
     <row r="163" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D163" s="56"/>
+      <c r="D163" s="40"/>
     </row>
     <row r="164" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D164" s="56"/>
+      <c r="D164" s="40"/>
     </row>
     <row r="165" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D165" s="56"/>
+      <c r="D165" s="40"/>
     </row>
     <row r="166" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D166" s="56"/>
+      <c r="D166" s="40"/>
     </row>
     <row r="167" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D167" s="56"/>
+      <c r="D167" s="40"/>
     </row>
     <row r="168" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D168" s="56"/>
+      <c r="D168" s="40"/>
     </row>
     <row r="169" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D169" s="56"/>
+      <c r="D169" s="40"/>
     </row>
     <row r="170" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D170" s="56"/>
+      <c r="D170" s="40"/>
     </row>
     <row r="171" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D171" s="56"/>
+      <c r="D171" s="40"/>
     </row>
     <row r="172" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D172" s="56"/>
+      <c r="D172" s="40"/>
     </row>
     <row r="173" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D173" s="56"/>
+      <c r="D173" s="40"/>
     </row>
     <row r="174" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D174" s="56"/>
+      <c r="D174" s="40"/>
     </row>
     <row r="175" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D175" s="56"/>
+      <c r="D175" s="40"/>
     </row>
     <row r="176" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D176" s="56"/>
+      <c r="D176" s="40"/>
     </row>
     <row r="177" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D177" s="56"/>
+      <c r="D177" s="40"/>
     </row>
     <row r="178" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D178" s="56"/>
+      <c r="D178" s="40"/>
     </row>
     <row r="179" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D179" s="56"/>
+      <c r="D179" s="40"/>
     </row>
     <row r="180" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D180" s="56"/>
+      <c r="D180" s="40"/>
     </row>
     <row r="181" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D181" s="56"/>
+      <c r="D181" s="40"/>
     </row>
     <row r="182" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D182" s="56"/>
+      <c r="D182" s="40"/>
     </row>
     <row r="183" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D183" s="56"/>
+      <c r="D183" s="40"/>
     </row>
     <row r="184" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D184" s="56"/>
+      <c r="D184" s="40"/>
     </row>
     <row r="185" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D185" s="56"/>
+      <c r="D185" s="40"/>
     </row>
     <row r="186" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D186" s="56"/>
+      <c r="D186" s="40"/>
     </row>
     <row r="187" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D187" s="56"/>
+      <c r="D187" s="40"/>
     </row>
     <row r="188" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D188" s="56"/>
+      <c r="D188" s="40"/>
     </row>
     <row r="189" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D189" s="56"/>
+      <c r="D189" s="40"/>
     </row>
     <row r="190" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D190" s="56"/>
+      <c r="D190" s="40"/>
     </row>
     <row r="191" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D191" s="56"/>
+      <c r="D191" s="40"/>
     </row>
     <row r="192" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D192" s="56"/>
+      <c r="D192" s="40"/>
     </row>
     <row r="193" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D193" s="56"/>
+      <c r="D193" s="40"/>
     </row>
     <row r="194" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D194" s="56"/>
+      <c r="D194" s="40"/>
     </row>
     <row r="195" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D195" s="56"/>
+      <c r="D195" s="40"/>
     </row>
     <row r="196" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D196" s="56"/>
+      <c r="D196" s="40"/>
     </row>
     <row r="197" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D197" s="56"/>
+      <c r="D197" s="40"/>
     </row>
     <row r="198" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D198" s="56"/>
+      <c r="D198" s="40"/>
     </row>
     <row r="199" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D199" s="56"/>
+      <c r="D199" s="40"/>
     </row>
     <row r="200" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D200" s="56"/>
+      <c r="D200" s="40"/>
     </row>
     <row r="201" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D201" s="56"/>
+      <c r="D201" s="40"/>
     </row>
     <row r="202" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D202" s="56"/>
+      <c r="D202" s="40"/>
     </row>
     <row r="203" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D203" s="56"/>
+      <c r="D203" s="40"/>
     </row>
     <row r="204" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D204" s="56"/>
+      <c r="D204" s="40"/>
     </row>
     <row r="205" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D205" s="56"/>
+      <c r="D205" s="40"/>
     </row>
     <row r="206" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D206" s="56"/>
+      <c r="D206" s="40"/>
     </row>
     <row r="207" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D207" s="56"/>
+      <c r="D207" s="40"/>
     </row>
     <row r="208" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D208" s="56"/>
+      <c r="D208" s="40"/>
     </row>
     <row r="209" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D209" s="56"/>
+      <c r="D209" s="40"/>
     </row>
     <row r="210" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D210" s="56"/>
+      <c r="D210" s="40"/>
     </row>
     <row r="211" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D211" s="56"/>
+      <c r="D211" s="40"/>
     </row>
     <row r="212" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D212" s="56"/>
+      <c r="D212" s="40"/>
     </row>
     <row r="213" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D213" s="56"/>
+      <c r="D213" s="40"/>
     </row>
     <row r="214" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D214" s="56"/>
+      <c r="D214" s="40"/>
     </row>
     <row r="215" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D215" s="56"/>
+      <c r="D215" s="40"/>
     </row>
     <row r="216" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D216" s="56"/>
+      <c r="D216" s="40"/>
     </row>
     <row r="217" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D217" s="56"/>
+      <c r="D217" s="40"/>
     </row>
     <row r="218" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D218" s="56"/>
+      <c r="D218" s="40"/>
     </row>
     <row r="219" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D219" s="56"/>
+      <c r="D219" s="40"/>
     </row>
     <row r="220" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D220" s="56"/>
+      <c r="D220" s="40"/>
     </row>
     <row r="221" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D221" s="56"/>
+      <c r="D221" s="40"/>
     </row>
     <row r="222" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D222" s="56"/>
+      <c r="D222" s="40"/>
     </row>
     <row r="223" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D223" s="56"/>
+      <c r="D223" s="40"/>
     </row>
     <row r="224" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D224" s="56"/>
+      <c r="D224" s="40"/>
     </row>
     <row r="225" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D225" s="56"/>
+      <c r="D225" s="40"/>
     </row>
     <row r="226" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D226" s="56"/>
+      <c r="D226" s="40"/>
     </row>
     <row r="227" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D227" s="56"/>
+      <c r="D227" s="40"/>
     </row>
     <row r="228" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D228" s="56"/>
+      <c r="D228" s="40"/>
     </row>
     <row r="229" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D229" s="56"/>
+      <c r="D229" s="40"/>
     </row>
     <row r="230" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D230" s="56"/>
+      <c r="D230" s="40"/>
     </row>
     <row r="231" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D231" s="56"/>
+      <c r="D231" s="40"/>
     </row>
     <row r="232" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D232" s="56"/>
+      <c r="D232" s="40"/>
     </row>
     <row r="233" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D233" s="56"/>
+      <c r="D233" s="40"/>
     </row>
     <row r="234" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D234" s="56"/>
+      <c r="D234" s="40"/>
     </row>
     <row r="235" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D235" s="56"/>
+      <c r="D235" s="40"/>
     </row>
     <row r="236" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D236" s="56"/>
+      <c r="D236" s="40"/>
     </row>
     <row r="237" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D237" s="56"/>
+      <c r="D237" s="40"/>
     </row>
     <row r="238" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D238" s="56"/>
+      <c r="D238" s="40"/>
     </row>
     <row r="239" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D239" s="56"/>
+      <c r="D239" s="40"/>
     </row>
     <row r="240" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D240" s="56"/>
+      <c r="D240" s="40"/>
     </row>
     <row r="241" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D241" s="56"/>
+      <c r="D241" s="40"/>
     </row>
     <row r="242" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D242" s="56"/>
+      <c r="D242" s="40"/>
     </row>
     <row r="243" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D243" s="56"/>
+      <c r="D243" s="40"/>
     </row>
     <row r="244" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D244" s="56"/>
+      <c r="D244" s="40"/>
     </row>
     <row r="245" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D245" s="56"/>
+      <c r="D245" s="40"/>
     </row>
     <row r="246" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D246" s="56"/>
+      <c r="D246" s="40"/>
     </row>
     <row r="247" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D247" s="56"/>
+      <c r="D247" s="40"/>
     </row>
     <row r="248" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D248" s="56"/>
+      <c r="D248" s="40"/>
     </row>
     <row r="249" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D249" s="56"/>
+      <c r="D249" s="40"/>
     </row>
     <row r="250" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D250" s="56"/>
+      <c r="D250" s="40"/>
     </row>
     <row r="251" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D251" s="56"/>
+      <c r="D251" s="40"/>
     </row>
     <row r="252" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D252" s="56"/>
+      <c r="D252" s="40"/>
     </row>
     <row r="253" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D253" s="56"/>
+      <c r="D253" s="40"/>
     </row>
     <row r="254" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D254" s="56"/>
+      <c r="D254" s="40"/>
     </row>
     <row r="255" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D255" s="56"/>
+      <c r="D255" s="40"/>
     </row>
     <row r="256" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D256" s="56"/>
+      <c r="D256" s="40"/>
     </row>
     <row r="257" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D257" s="56"/>
+      <c r="D257" s="40"/>
     </row>
     <row r="258" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D258" s="56"/>
+      <c r="D258" s="40"/>
     </row>
     <row r="259" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D259" s="56"/>
+      <c r="D259" s="40"/>
     </row>
     <row r="260" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D260" s="56"/>
+      <c r="D260" s="40"/>
     </row>
     <row r="261" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D261" s="56"/>
+      <c r="D261" s="40"/>
     </row>
     <row r="262" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D262" s="56"/>
+      <c r="D262" s="40"/>
     </row>
     <row r="263" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D263" s="56"/>
+      <c r="D263" s="40"/>
     </row>
     <row r="264" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D264" s="56"/>
+      <c r="D264" s="40"/>
     </row>
     <row r="265" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D265" s="56"/>
+      <c r="D265" s="40"/>
     </row>
     <row r="266" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D266" s="56"/>
+      <c r="D266" s="40"/>
     </row>
     <row r="267" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D267" s="56"/>
+      <c r="D267" s="40"/>
     </row>
     <row r="268" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D268" s="56"/>
+      <c r="D268" s="40"/>
     </row>
     <row r="269" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D269" s="56"/>
+      <c r="D269" s="40"/>
     </row>
     <row r="270" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D270" s="56"/>
+      <c r="D270" s="40"/>
     </row>
     <row r="271" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D271" s="56"/>
+      <c r="D271" s="40"/>
     </row>
     <row r="272" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D272" s="56"/>
+      <c r="D272" s="40"/>
     </row>
     <row r="273" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D273" s="56"/>
+      <c r="D273" s="40"/>
     </row>
     <row r="274" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D274" s="56"/>
+      <c r="D274" s="40"/>
     </row>
     <row r="275" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D275" s="56"/>
+      <c r="D275" s="40"/>
     </row>
     <row r="276" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D276" s="56"/>
+      <c r="D276" s="40"/>
     </row>
     <row r="277" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D277" s="56"/>
+      <c r="D277" s="40"/>
     </row>
     <row r="278" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D278" s="56"/>
+      <c r="D278" s="40"/>
     </row>
     <row r="279" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D279" s="56"/>
+      <c r="D279" s="40"/>
     </row>
     <row r="280" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D280" s="56"/>
+      <c r="D280" s="40"/>
     </row>
     <row r="281" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D281" s="56"/>
+      <c r="D281" s="40"/>
     </row>
     <row r="282" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D282" s="56"/>
+      <c r="D282" s="40"/>
     </row>
     <row r="283" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D283" s="56"/>
+      <c r="D283" s="40"/>
     </row>
     <row r="284" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D284" s="56"/>
+      <c r="D284" s="40"/>
     </row>
     <row r="285" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D285" s="56"/>
+      <c r="D285" s="40"/>
     </row>
     <row r="286" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D286" s="56"/>
+      <c r="D286" s="40"/>
     </row>
     <row r="287" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D287" s="56"/>
+      <c r="D287" s="40"/>
     </row>
     <row r="288" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D288" s="56"/>
+      <c r="D288" s="40"/>
     </row>
     <row r="289" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D289" s="56"/>
+      <c r="D289" s="40"/>
     </row>
     <row r="290" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D290" s="56"/>
+      <c r="D290" s="40"/>
     </row>
     <row r="291" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D291" s="56"/>
+      <c r="D291" s="40"/>
     </row>
     <row r="292" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D292" s="56"/>
+      <c r="D292" s="40"/>
     </row>
     <row r="293" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D293" s="56"/>
+      <c r="D293" s="40"/>
     </row>
     <row r="294" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D294" s="56"/>
+      <c r="D294" s="40"/>
     </row>
     <row r="295" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D295" s="56"/>
+      <c r="D295" s="40"/>
     </row>
     <row r="296" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D296" s="56"/>
+      <c r="D296" s="40"/>
     </row>
     <row r="297" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D297" s="56"/>
+      <c r="D297" s="40"/>
     </row>
     <row r="298" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D298" s="56"/>
+      <c r="D298" s="40"/>
     </row>
     <row r="299" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D299" s="56"/>
+      <c r="D299" s="40"/>
     </row>
     <row r="300" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D300" s="56"/>
+      <c r="D300" s="40"/>
     </row>
     <row r="301" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D301" s="56"/>
+      <c r="D301" s="40"/>
     </row>
     <row r="302" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D302" s="56"/>
+      <c r="D302" s="40"/>
     </row>
     <row r="303" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D303" s="56"/>
+      <c r="D303" s="40"/>
     </row>
     <row r="304" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D304" s="56"/>
+      <c r="D304" s="40"/>
     </row>
     <row r="305" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D305" s="56"/>
+      <c r="D305" s="40"/>
     </row>
     <row r="306" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D306" s="56"/>
+      <c r="D306" s="40"/>
     </row>
     <row r="307" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D307" s="56"/>
+      <c r="D307" s="40"/>
     </row>
     <row r="308" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D308" s="56"/>
+      <c r="D308" s="40"/>
     </row>
     <row r="309" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D309" s="56"/>
+      <c r="D309" s="40"/>
     </row>
     <row r="310" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D310" s="56"/>
+      <c r="D310" s="40"/>
     </row>
     <row r="311" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D311" s="56"/>
+      <c r="D311" s="40"/>
     </row>
     <row r="312" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D312" s="56"/>
+      <c r="D312" s="40"/>
     </row>
     <row r="313" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D313" s="56"/>
+      <c r="D313" s="40"/>
     </row>
     <row r="314" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D314" s="56"/>
+      <c r="D314" s="40"/>
     </row>
     <row r="315" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D315" s="56"/>
+      <c r="D315" s="40"/>
     </row>
     <row r="316" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D316" s="56"/>
+      <c r="D316" s="40"/>
     </row>
     <row r="317" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D317" s="56"/>
+      <c r="D317" s="40"/>
     </row>
     <row r="318" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D318" s="56"/>
+      <c r="D318" s="40"/>
     </row>
     <row r="319" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D319" s="56"/>
+      <c r="D319" s="40"/>
     </row>
     <row r="320" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D320" s="56"/>
+      <c r="D320" s="40"/>
     </row>
     <row r="321" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D321" s="56"/>
+      <c r="D321" s="40"/>
     </row>
     <row r="322" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D322" s="56"/>
+      <c r="D322" s="40"/>
     </row>
     <row r="323" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D323" s="56"/>
+      <c r="D323" s="40"/>
     </row>
     <row r="324" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D324" s="56"/>
+      <c r="D324" s="40"/>
     </row>
     <row r="325" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D325" s="56"/>
+      <c r="D325" s="40"/>
     </row>
     <row r="326" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D326" s="56"/>
+      <c r="D326" s="40"/>
     </row>
     <row r="327" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D327" s="56"/>
+      <c r="D327" s="40"/>
     </row>
     <row r="328" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D328" s="56"/>
+      <c r="D328" s="40"/>
     </row>
     <row r="329" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D329" s="56"/>
+      <c r="D329" s="40"/>
     </row>
     <row r="330" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D330" s="56"/>
+      <c r="D330" s="40"/>
     </row>
     <row r="331" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D331" s="56"/>
+      <c r="D331" s="40"/>
     </row>
     <row r="332" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D332" s="56"/>
+      <c r="D332" s="40"/>
     </row>
     <row r="333" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D333" s="56"/>
+      <c r="D333" s="40"/>
     </row>
     <row r="334" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D334" s="56"/>
+      <c r="D334" s="40"/>
     </row>
     <row r="335" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D335" s="56"/>
+      <c r="D335" s="40"/>
     </row>
     <row r="336" spans="4:4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D336" s="56"/>
+      <c r="D336" s="40"/>
     </row>
     <row r="337" ht="15" x14ac:dyDescent="0.25"/>
     <row r="338" ht="15" x14ac:dyDescent="0.25"/>
     <row r="339" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="340" ht="15" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="D3:D5"/>
-    <mergeCell ref="D6:D8"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="D20:D22"/>
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="D14:D16"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3889,8 +3932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD6B0F65-C746-424A-8F79-B872BB8F9443}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3904,16 +3947,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="62" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="F1" s="43" t="s">
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="F1" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="G1" s="43"/>
+      <c r="G1" s="58"/>
     </row>
     <row r="2" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="28" t="s">
@@ -3939,18 +3982,18 @@
       <c r="A3" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="61">
+      <c r="B3" s="45">
         <f>F3</f>
         <v>21</v>
       </c>
-      <c r="C3" s="61">
+      <c r="C3" s="45">
         <f>F3</f>
         <v>21</v>
       </c>
-      <c r="D3" s="62">
+      <c r="D3" s="46">
         <v>44119</v>
       </c>
-      <c r="F3" s="60">
+      <c r="F3" s="44">
         <f>COUNTA(Sprints!B3:B23)</f>
         <v>21</v>
       </c>
@@ -3968,7 +4011,7 @@
         <v>18.375</v>
       </c>
       <c r="C4" s="30"/>
-      <c r="D4" s="47">
+      <c r="D4" s="37">
         <f>Sprints!D3</f>
         <v>44121</v>
       </c>
@@ -3982,8 +4025,8 @@
         <v>15.75</v>
       </c>
       <c r="C5" s="30"/>
-      <c r="D5" s="47">
-        <f>Sprints!D6</f>
+      <c r="D5" s="37">
+        <f>Sprints!D5</f>
         <v>44123</v>
       </c>
     </row>
@@ -3996,8 +4039,8 @@
         <v>13.125</v>
       </c>
       <c r="C6" s="30"/>
-      <c r="D6" s="47">
-        <f>Sprints!D9</f>
+      <c r="D6" s="37">
+        <f>Sprints!D8</f>
         <v>44125</v>
       </c>
     </row>
@@ -4010,8 +4053,8 @@
         <v>10.5</v>
       </c>
       <c r="C7" s="30"/>
-      <c r="D7" s="47">
-        <f>Sprints!D12</f>
+      <c r="D7" s="37">
+        <f>Sprints!D11</f>
         <v>44127</v>
       </c>
     </row>
@@ -4024,8 +4067,8 @@
         <v>7.875</v>
       </c>
       <c r="C8" s="30"/>
-      <c r="D8" s="47">
-        <f>Sprints!D15</f>
+      <c r="D8" s="37">
+        <f>Sprints!D14</f>
         <v>44129</v>
       </c>
     </row>
@@ -4038,8 +4081,8 @@
         <v>5.25</v>
       </c>
       <c r="C9" s="30"/>
-      <c r="D9" s="47">
-        <f>Sprints!D18</f>
+      <c r="D9" s="37">
+        <f>Sprints!D17</f>
         <v>44131</v>
       </c>
     </row>
@@ -4052,8 +4095,8 @@
         <v>2.625</v>
       </c>
       <c r="C10" s="30"/>
-      <c r="D10" s="47">
-        <f>Sprints!D21</f>
+      <c r="D10" s="37">
+        <f>Sprints!D20</f>
         <v>44133</v>
       </c>
     </row>
@@ -4066,7 +4109,7 @@
         <v>0</v>
       </c>
       <c r="C11" s="30"/>
-      <c r="D11" s="47">
+      <c r="D11" s="37">
         <f>Sprints!D23</f>
         <v>44135</v>
       </c>
@@ -4076,25 +4119,25 @@
       <c r="A13" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="B13" s="63">
+      <c r="B13" s="60">
         <v>43997</v>
       </c>
-      <c r="C13" s="64"/>
+      <c r="C13" s="61"/>
     </row>
     <row r="14" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="B14" s="63" t="s">
+      <c r="B14" s="60" t="s">
         <v>80</v>
       </c>
-      <c r="C14" s="64"/>
+      <c r="C14" s="61"/>
     </row>
     <row r="15" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="44" t="s">
+      <c r="A15" s="59" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="44"/>
+      <c r="B15" s="59"/>
       <c r="C15" s="34"/>
     </row>
   </sheetData>

</xml_diff>